<commit_message>
thresholded and preprocessed data sessions 20240119 and 20240112
</commit_message>
<xml_diff>
--- a/ExcelFiles/s3_good_trials_GraspObject_Shuffled.xlsx
+++ b/ExcelFiles/s3_good_trials_GraspObject_Shuffled.xlsx
@@ -8,20 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\macthurston\Documents\GitHub\project_grasp_object_interaction\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93F72734-82B6-46E4-9CA0-1520C062FF21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E815652-E7FB-47FF-AF55-29719972330C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="765" yWindow="11310" windowWidth="14115" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="990" yWindow="300" windowWidth="14115" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="8">
   <si>
     <t>Date</t>
   </si>
@@ -42,6 +41,9 @@
   </si>
   <si>
     <t>32 trials</t>
+  </si>
+  <si>
+    <t>24 trials--&gt;</t>
   </si>
 </sst>
 </file>
@@ -360,10 +362,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,6 +481,57 @@
         <v>5</v>
       </c>
     </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>20240112</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>20240119</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>6</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>